<commit_message>
Kristina made me change a bunch of shit for allotted hours
Allotted hours actually means default runtime for LF, 2pk etc, not
planned. Now everything is average title multiplied by whatever.
</commit_message>
<xml_diff>
--- a/tables/allotted_hours.xlsx
+++ b/tables/allotted_hours.xlsx
@@ -17,8 +17,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="H49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Saw very little but it looks legit</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="188">
   <si>
     <t>mso</t>
   </si>
@@ -461,9 +495,6 @@
     <t>Adam &amp; Eve</t>
   </si>
   <si>
-    <t>Club Taboo</t>
-  </si>
-  <si>
     <t>High Society</t>
   </si>
   <si>
@@ -506,18 +537,12 @@
     <t>Girl Crush SD&amp;HD Hours added</t>
   </si>
   <si>
-    <t>Vivid Gay Hours added</t>
-  </si>
-  <si>
     <t>Babes HD hours added</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>Don't see in 2016</t>
-  </si>
-  <si>
     <t>provider</t>
   </si>
   <si>
@@ -585,13 +610,19 @@
   </si>
   <si>
     <t>Forbidden Fruits HD</t>
+  </si>
+  <si>
+    <t>Girl Crush HD</t>
+  </si>
+  <si>
+    <t>Rolled up Vivid 2pk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +667,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -788,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -852,9 +896,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,62 +928,37 @@
     <xf numFmtId="1" fontId="5" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
@@ -957,51 +973,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1029,7 +1000,58 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1054,6 +1076,50 @@
           <color rgb="FF95B3D7"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -6222,8 +6288,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="titles_trend" displayName="titles_trend" ref="A1:N307" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="13">
-  <autoFilter ref="A1:N307">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="titles_trend" displayName="titles_trend" ref="A1:N308" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10">
+  <autoFilter ref="A1:N308">
     <filterColumn colId="0">
       <filters>
         <filter val="Cablevision"/>
@@ -6236,16 +6302,16 @@
     <sortCondition ref="C2:C301"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="mso" dataDxfId="12"/>
+    <tableColumn id="1" name="mso" dataDxfId="9"/>
     <tableColumn id="6" name="offering" dataDxfId="8"/>
     <tableColumn id="2" name="offering_rollup"/>
-    <tableColumn id="4" name="provider" dataDxfId="11">
+    <tableColumn id="4" name="provider" dataDxfId="7">
       <calculatedColumnFormula>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="type" dataDxfId="2">
+    <tableColumn id="5" name="type" dataDxfId="6">
       <calculatedColumnFormula>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="default_hours" dataDxfId="4">
+    <tableColumn id="7" name="default_hours" dataDxfId="5">
       <calculatedColumnFormula>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="notes"/>
@@ -6262,14 +6328,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <sortState ref="A2:B9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="type" dataDxfId="10"/>
-    <tableColumn id="3" name="mins" dataDxfId="6"/>
-    <tableColumn id="2" name="hours" dataDxfId="5">
+    <tableColumn id="1" name="type" dataDxfId="2"/>
+    <tableColumn id="3" name="mins" dataDxfId="1"/>
+    <tableColumn id="2" name="hours" dataDxfId="0">
       <calculatedColumnFormula>Table3[[#This Row],[mins]]/60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6563,15 +6629,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N307"/>
+  <dimension ref="A1:P308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6585,7 +6651,7 @@
     <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="9.140625" style="25"/>
-    <col min="14" max="14" width="9.140625" style="37"/>
+    <col min="14" max="14" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6596,40 +6662,40 @@
         <v>144</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>158</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -7344,7 +7410,7 @@
       <c r="M26" s="25">
         <v>14</v>
       </c>
-      <c r="N26" s="37">
+      <c r="N26" s="36">
         <v>14</v>
       </c>
     </row>
@@ -7388,7 +7454,7 @@
       <c r="M27" s="25">
         <v>12</v>
       </c>
-      <c r="N27" s="37">
+      <c r="N27" s="36">
         <v>12</v>
       </c>
     </row>
@@ -7432,7 +7498,7 @@
       <c r="M28" s="25">
         <v>4</v>
       </c>
-      <c r="N28" s="37">
+      <c r="N28" s="36">
         <v>4</v>
       </c>
     </row>
@@ -7476,7 +7542,7 @@
       <c r="M29" s="25">
         <v>4</v>
       </c>
-      <c r="N29" s="37">
+      <c r="N29" s="36">
         <v>4</v>
       </c>
     </row>
@@ -7520,7 +7586,7 @@
       <c r="M30" s="25">
         <v>10</v>
       </c>
-      <c r="N30" s="37">
+      <c r="N30" s="36">
         <v>10</v>
       </c>
     </row>
@@ -7564,7 +7630,7 @@
       <c r="M31" s="25">
         <v>8</v>
       </c>
-      <c r="N31" s="37">
+      <c r="N31" s="36">
         <v>8</v>
       </c>
     </row>
@@ -7591,7 +7657,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H32" s="26">
         <v>36</v>
@@ -7611,7 +7677,7 @@
       <c r="M32" s="26">
         <v>36</v>
       </c>
-      <c r="N32" s="38">
+      <c r="N32" s="37">
         <v>36</v>
       </c>
     </row>
@@ -7656,7 +7722,7 @@
       <c r="M33" s="28">
         <v>6</v>
       </c>
-      <c r="N33" s="39">
+      <c r="N33" s="38">
         <v>6</v>
       </c>
     </row>
@@ -7700,7 +7766,7 @@
       <c r="M34" s="29">
         <v>16</v>
       </c>
-      <c r="N34" s="40">
+      <c r="N34" s="39">
         <v>16</v>
       </c>
     </row>
@@ -7727,7 +7793,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="27"/>
@@ -7735,14 +7801,14 @@
       <c r="K35" s="27"/>
       <c r="L35" s="27"/>
       <c r="M35" s="27"/>
-      <c r="N35" s="41"/>
+      <c r="N35" s="40"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>21</v>
@@ -7752,7 +7818,7 @@
         <v>Hustler</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F36" s="20">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
@@ -7777,7 +7843,7 @@
       <c r="M36" s="30">
         <v>12</v>
       </c>
-      <c r="N36" s="42">
+      <c r="N36" s="41">
         <v>12</v>
       </c>
     </row>
@@ -7786,7 +7852,7 @@
         <v>24</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>21</v>
@@ -7796,7 +7862,7 @@
         <v>Hustler</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F37" s="20">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
@@ -7821,7 +7887,7 @@
       <c r="M37" s="30">
         <v>18</v>
       </c>
-      <c r="N37" s="42">
+      <c r="N37" s="41">
         <v>18</v>
       </c>
     </row>
@@ -7866,7 +7932,7 @@
       <c r="M38" s="31">
         <v>18</v>
       </c>
-      <c r="N38" s="43">
+      <c r="N38" s="42">
         <v>22</v>
       </c>
     </row>
@@ -7893,7 +7959,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="27"/>
@@ -7901,24 +7967,24 @@
       <c r="K39" s="27"/>
       <c r="L39" s="27"/>
       <c r="M39" s="27"/>
-      <c r="N39" s="41"/>
+      <c r="N39" s="40"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="34" t="str">
+      <c r="D40" s="33" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>Hustler</v>
       </c>
-      <c r="E40" s="34" t="s">
-        <v>172</v>
+      <c r="E40" s="33" t="s">
+        <v>169</v>
       </c>
       <c r="F40" s="20">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
@@ -7926,20 +7992,20 @@
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="30"/>
-      <c r="I40" s="35">
+      <c r="I40" s="34">
         <v>1</v>
       </c>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35">
+      <c r="J40" s="34"/>
+      <c r="K40" s="34">
         <v>3</v>
       </c>
-      <c r="L40" s="35">
+      <c r="L40" s="34">
         <v>3</v>
       </c>
-      <c r="M40" s="35">
+      <c r="M40" s="34">
         <v>6</v>
       </c>
-      <c r="N40" s="44">
+      <c r="N40" s="43">
         <v>6</v>
       </c>
     </row>
@@ -7948,17 +8014,17 @@
         <v>24</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="34" t="str">
+      <c r="D41" s="33" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>Hustler</v>
       </c>
-      <c r="E41" s="34" t="s">
-        <v>172</v>
+      <c r="E41" s="33" t="s">
+        <v>169</v>
       </c>
       <c r="F41" s="20">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
@@ -7966,20 +8032,20 @@
       </c>
       <c r="G41" s="19"/>
       <c r="H41" s="30"/>
-      <c r="I41" s="35">
+      <c r="I41" s="34">
         <v>8</v>
       </c>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35">
+      <c r="J41" s="34"/>
+      <c r="K41" s="34">
         <v>3</v>
       </c>
-      <c r="L41" s="35">
+      <c r="L41" s="34">
         <v>3</v>
       </c>
-      <c r="M41" s="35">
+      <c r="M41" s="34">
         <v>6</v>
       </c>
-      <c r="N41" s="44">
+      <c r="N41" s="43">
         <v>6</v>
       </c>
     </row>
@@ -7993,11 +8059,11 @@
       <c r="C42" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="36" t="str">
+      <c r="D42" s="35" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>Hustler</v>
       </c>
-      <c r="E42" s="36" t="str">
+      <c r="E42" s="35" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
         <v>LF</v>
       </c>
@@ -8024,7 +8090,7 @@
       <c r="M42" s="31">
         <v>16</v>
       </c>
-      <c r="N42" s="45">
+      <c r="N42" s="44">
         <v>16</v>
       </c>
     </row>
@@ -8051,7 +8117,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H43" s="25">
         <v>8</v>
@@ -8071,7 +8137,7 @@
       <c r="M43" s="32">
         <v>8</v>
       </c>
-      <c r="N43" s="40">
+      <c r="N43" s="39">
         <v>8</v>
       </c>
     </row>
@@ -8098,7 +8164,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H44" s="25">
         <v>12</v>
@@ -8116,10 +8182,10 @@
         <v>16</v>
       </c>
       <c r="M44" s="32">
-        <v>18</v>
-      </c>
-      <c r="N44" s="40">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="N44" s="32">
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -8144,14 +8210,11 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G45" t="s">
-        <v>169</v>
-      </c>
       <c r="H45" s="25">
         <v>12</v>
       </c>
       <c r="I45" s="32">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J45" s="32">
         <v>48</v>
@@ -8165,7 +8228,7 @@
       <c r="M45" s="32">
         <v>38</v>
       </c>
-      <c r="N45" s="40">
+      <c r="N45" s="39">
         <v>38</v>
       </c>
     </row>
@@ -8200,7 +8263,7 @@
       <c r="M46" s="32">
         <v>15</v>
       </c>
-      <c r="N46" s="40">
+      <c r="N46" s="39">
         <v>15</v>
       </c>
     </row>
@@ -8244,7 +8307,7 @@
       <c r="M47" s="29">
         <v>24</v>
       </c>
-      <c r="N47" s="40">
+      <c r="N47" s="39">
         <v>24</v>
       </c>
     </row>
@@ -8271,7 +8334,7 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="G48" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H48" s="25">
         <v>12</v>
@@ -8291,11 +8354,11 @@
       <c r="M48" s="29">
         <v>24</v>
       </c>
-      <c r="N48" s="40">
+      <c r="N48" s="39">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
@@ -8330,110 +8393,150 @@
         <v>18</v>
       </c>
       <c r="L49" s="29">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M49" s="29">
         <v>20</v>
       </c>
-      <c r="N49" s="40">
+      <c r="N49" s="39">
         <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D50" t="str">
+      <c r="D50" s="16" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>TVN</v>
       </c>
-      <c r="E50" t="str">
+      <c r="E50" s="16" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
         <v>LF</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="17">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G50" t="s">
-        <v>161</v>
-      </c>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="40"/>
+      <c r="G50" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H50" s="26">
+        <v>20</v>
+      </c>
+      <c r="I50" s="26">
+        <v>25</v>
+      </c>
+      <c r="J50" s="26">
+        <v>20</v>
+      </c>
+      <c r="K50" s="26">
+        <v>20</v>
+      </c>
+      <c r="L50" s="26">
+        <v>20</v>
+      </c>
+      <c r="M50" s="26">
+        <v>20</v>
+      </c>
+      <c r="N50" s="52">
+        <v>20</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C51" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" t="str">
+      <c r="B51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="54" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>TVN</v>
       </c>
-      <c r="E51" t="str">
+      <c r="E51" s="54" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
         <v>LF</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="55">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G51" t="s">
-        <v>165</v>
-      </c>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="33"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="G51" s="54"/>
+      <c r="H51" s="56">
+        <v>14</v>
+      </c>
+      <c r="I51" s="56">
+        <v>14</v>
+      </c>
+      <c r="J51" s="56">
+        <v>14</v>
+      </c>
+      <c r="K51" s="56">
+        <v>14</v>
+      </c>
+      <c r="L51" s="56">
+        <v>14</v>
+      </c>
+      <c r="M51" s="56">
+        <v>14</v>
+      </c>
+      <c r="N51" s="57">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" t="str">
+      <c r="B52" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="47" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>TVN</v>
       </c>
-      <c r="E52" t="str">
-        <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>LF</v>
-      </c>
-      <c r="F52" s="10">
+      <c r="E52" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="F52" s="48">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
+      <c r="G52" s="47"/>
+      <c r="H52" s="49">
+        <v>1</v>
+      </c>
+      <c r="I52" s="50">
+        <v>1</v>
+      </c>
+      <c r="J52" s="50"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="51"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="D53" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8446,6 +8549,27 @@
       <c r="F53" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
+      </c>
+      <c r="H53" s="25">
+        <v>12</v>
+      </c>
+      <c r="I53" s="25">
+        <v>12</v>
+      </c>
+      <c r="J53" s="25">
+        <v>8</v>
+      </c>
+      <c r="K53" s="25">
+        <v>8</v>
+      </c>
+      <c r="L53" s="25">
+        <v>8</v>
+      </c>
+      <c r="M53" s="25">
+        <v>8</v>
+      </c>
+      <c r="N53" s="25">
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -8453,14 +8577,14 @@
         <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D54" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Vivid</v>
+        <v>TVN</v>
       </c>
       <c r="E54" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8470,22 +8594,19 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="32"/>
-      <c r="N54" s="40"/>
+      <c r="N54" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D55" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8493,28 +8614,43 @@
       </c>
       <c r="E55" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>NW LF</v>
+        <v>LF</v>
       </c>
       <c r="F55" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="40"/>
+      <c r="H55" s="25">
+        <v>12</v>
+      </c>
+      <c r="I55" s="25">
+        <v>12</v>
+      </c>
+      <c r="J55" s="25">
+        <v>12</v>
+      </c>
+      <c r="K55" s="25">
+        <v>12</v>
+      </c>
+      <c r="L55" s="25">
+        <v>12</v>
+      </c>
+      <c r="M55" s="25">
+        <v>12</v>
+      </c>
+      <c r="N55" s="25">
+        <v>12</v>
+      </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D56" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8522,28 +8658,32 @@
       </c>
       <c r="E56" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>LF</v>
+        <v>NW LF</v>
       </c>
       <c r="F56" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I56" s="29"/>
-      <c r="J56" s="29"/>
-      <c r="K56" s="29"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="29"/>
-      <c r="N56" s="40"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32">
+        <v>3</v>
+      </c>
+      <c r="L56" s="32">
+        <v>3</v>
+      </c>
+      <c r="M56" s="32"/>
+      <c r="N56" s="39"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D57" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8557,22 +8697,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I57" s="29"/>
-      <c r="J57" s="29"/>
-      <c r="K57" s="29"/>
-      <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
-      <c r="N57" s="40"/>
+      <c r="H57" s="25">
+        <v>14</v>
+      </c>
+      <c r="I57" s="25">
+        <v>14</v>
+      </c>
+      <c r="J57" s="25">
+        <v>14</v>
+      </c>
+      <c r="K57" s="25">
+        <v>14</v>
+      </c>
+      <c r="L57" s="25">
+        <v>14</v>
+      </c>
+      <c r="M57" s="25">
+        <v>14</v>
+      </c>
+      <c r="N57" s="25">
+        <v>14</v>
+      </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D58" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8586,22 +8741,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
-      <c r="L58" s="29"/>
-      <c r="M58" s="29"/>
-      <c r="N58" s="40"/>
+      <c r="H58" s="25">
+        <v>4</v>
+      </c>
+      <c r="I58" s="29">
+        <v>4</v>
+      </c>
+      <c r="J58" s="29">
+        <v>7</v>
+      </c>
+      <c r="K58" s="29">
+        <v>4</v>
+      </c>
+      <c r="L58" s="29">
+        <v>4</v>
+      </c>
+      <c r="M58" s="29">
+        <v>4</v>
+      </c>
+      <c r="N58" s="39">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D59" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8615,22 +8785,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I59" s="29"/>
-      <c r="J59" s="29"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="29"/>
-      <c r="M59" s="29"/>
-      <c r="N59" s="40"/>
+      <c r="H59" s="29">
+        <v>30</v>
+      </c>
+      <c r="I59" s="29">
+        <v>30</v>
+      </c>
+      <c r="J59" s="29">
+        <v>30</v>
+      </c>
+      <c r="K59" s="29">
+        <v>30</v>
+      </c>
+      <c r="L59" s="29">
+        <v>30</v>
+      </c>
+      <c r="M59" s="29">
+        <v>30</v>
+      </c>
+      <c r="N59" s="29">
+        <v>30</v>
+      </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="D60" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8644,22 +8829,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="40"/>
+      <c r="H60" s="29">
+        <v>6</v>
+      </c>
+      <c r="I60" s="29">
+        <v>6</v>
+      </c>
+      <c r="J60" s="29">
+        <v>6</v>
+      </c>
+      <c r="K60" s="29">
+        <v>6</v>
+      </c>
+      <c r="L60" s="29">
+        <v>6</v>
+      </c>
+      <c r="M60" s="29">
+        <v>9</v>
+      </c>
+      <c r="N60" s="39">
+        <v>9</v>
+      </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8674,21 +8874,31 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="29"/>
-      <c r="N61" s="40"/>
+      <c r="J61" s="29">
+        <v>12</v>
+      </c>
+      <c r="K61" s="29">
+        <v>12</v>
+      </c>
+      <c r="L61" s="29">
+        <v>12</v>
+      </c>
+      <c r="M61" s="29">
+        <v>12</v>
+      </c>
+      <c r="N61" s="29">
+        <v>12</v>
+      </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="D62" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8701,6 +8911,22 @@
       <c r="F62" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
+      </c>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29">
+        <v>8</v>
+      </c>
+      <c r="K62" s="29">
+        <v>8</v>
+      </c>
+      <c r="L62" s="29">
+        <v>8</v>
+      </c>
+      <c r="M62" s="29">
+        <v>8</v>
+      </c>
+      <c r="N62" s="29">
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -8708,10 +8934,10 @@
         <v>24</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="D63" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8725,22 +8951,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I63" s="29"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="29"/>
-      <c r="L63" s="29"/>
-      <c r="M63" s="29"/>
-      <c r="N63" s="40"/>
+      <c r="H63" s="25">
+        <v>18</v>
+      </c>
+      <c r="I63" s="25">
+        <v>14</v>
+      </c>
+      <c r="J63" s="25">
+        <v>14</v>
+      </c>
+      <c r="K63" s="25">
+        <v>14</v>
+      </c>
+      <c r="L63" s="25">
+        <v>14</v>
+      </c>
+      <c r="M63" s="25">
+        <v>14</v>
+      </c>
+      <c r="N63" s="25">
+        <v>14</v>
+      </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D64" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8753,23 +8994,30 @@
       <c r="F64" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
+      </c>
+      <c r="H64" s="25">
+        <v>3</v>
       </c>
       <c r="I64" s="29"/>
       <c r="J64" s="29"/>
       <c r="K64" s="29"/>
       <c r="L64" s="29"/>
-      <c r="M64" s="29"/>
-      <c r="N64" s="40"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M64" s="29">
+        <v>3</v>
+      </c>
+      <c r="N64" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="D65" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8783,22 +9031,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
-      <c r="N65" s="40"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H65" s="32">
+        <v>16</v>
+      </c>
+      <c r="I65" s="32">
+        <v>16</v>
+      </c>
+      <c r="J65" s="32">
+        <v>16</v>
+      </c>
+      <c r="K65" s="32">
+        <v>16</v>
+      </c>
+      <c r="L65" s="32">
+        <v>16</v>
+      </c>
+      <c r="M65" s="32">
+        <v>16</v>
+      </c>
+      <c r="N65" s="39">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D66" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8812,22 +9075,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I66" s="29"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="29"/>
-      <c r="M66" s="29"/>
-      <c r="N66" s="40"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H66" s="25">
+        <v>8</v>
+      </c>
+      <c r="I66" s="29">
+        <v>4</v>
+      </c>
+      <c r="J66" s="29">
+        <v>8</v>
+      </c>
+      <c r="K66" s="29">
+        <v>6</v>
+      </c>
+      <c r="L66" s="29">
+        <v>5.5</v>
+      </c>
+      <c r="M66" s="29">
+        <v>4</v>
+      </c>
+      <c r="N66" s="39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C67" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D67" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8841,22 +9119,37 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="29"/>
-      <c r="M67" s="29"/>
-      <c r="N67" s="40"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H67" s="25">
+        <v>12</v>
+      </c>
+      <c r="I67" s="25">
+        <v>12</v>
+      </c>
+      <c r="J67" s="25">
+        <v>12</v>
+      </c>
+      <c r="K67" s="25">
+        <v>12</v>
+      </c>
+      <c r="L67" s="25">
+        <v>12</v>
+      </c>
+      <c r="M67" s="25">
+        <v>12</v>
+      </c>
+      <c r="N67" s="25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D68" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -8870,165 +9163,245 @@
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G68" t="s">
-        <v>162</v>
+      <c r="H68" s="25">
+        <v>3</v>
       </c>
       <c r="I68" s="29"/>
       <c r="J68" s="29"/>
       <c r="K68" s="29"/>
       <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="40"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="M68" s="29">
+        <v>3</v>
+      </c>
+      <c r="N68" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="16" t="str">
+        <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
+        <v>Vivid</v>
+      </c>
+      <c r="E69" s="16" t="str">
+        <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
+        <v>LF</v>
+      </c>
+      <c r="F69" s="17">
+        <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H69" s="26">
+        <v>50</v>
+      </c>
+      <c r="I69" s="27">
+        <v>60</v>
+      </c>
+      <c r="J69" s="27">
+        <v>60</v>
+      </c>
+      <c r="K69" s="26">
+        <v>50</v>
+      </c>
+      <c r="L69" s="26">
+        <v>50</v>
+      </c>
+      <c r="M69" s="26">
+        <v>50</v>
+      </c>
+      <c r="N69" s="52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="C69" t="s">
-        <v>79</v>
-      </c>
-      <c r="D69" t="str">
+      <c r="C70" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="47" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>Vivid</v>
       </c>
-      <c r="E69" t="str">
+      <c r="E70" s="47" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
         <v>2PK</v>
       </c>
-      <c r="F69" s="10">
+      <c r="F70" s="48">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>2.6666666666666665</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C70" t="s">
-        <v>66</v>
-      </c>
-      <c r="D70" t="str">
-        <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Vivid</v>
-      </c>
-      <c r="E70" t="str">
-        <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>LF</v>
-      </c>
-      <c r="F70" s="10">
-        <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
-      <c r="K70" s="29"/>
-      <c r="L70" s="29"/>
-      <c r="M70" s="29"/>
-      <c r="N70" s="40"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G70" s="47"/>
+      <c r="H70" s="49">
+        <v>1</v>
+      </c>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="49"/>
+      <c r="L70" s="49"/>
+      <c r="M70" s="49"/>
+      <c r="N70" s="51"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" t="str">
+        <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
+        <v>Vivid</v>
+      </c>
+      <c r="E71" t="str">
+        <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
+        <v>LF</v>
+      </c>
+      <c r="F71" s="10">
+        <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="H71" s="29">
+        <v>18</v>
+      </c>
+      <c r="I71" s="29">
+        <v>18</v>
+      </c>
+      <c r="J71" s="29">
+        <v>18</v>
+      </c>
+      <c r="K71" s="29">
+        <v>18</v>
+      </c>
+      <c r="L71" s="29">
+        <v>18</v>
+      </c>
+      <c r="M71" s="29">
+        <v>18</v>
+      </c>
+      <c r="N71" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>33</v>
       </c>
-      <c r="D71" t="str">
+      <c r="D72" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>Vivid</v>
       </c>
-      <c r="E71" t="str">
+      <c r="E72" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
         <v>LF</v>
       </c>
-      <c r="F71" s="10">
+      <c r="F72" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
-      <c r="K71" s="29"/>
-      <c r="L71" s="29"/>
-      <c r="M71" s="29"/>
-      <c r="N71" s="40"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="H72" s="29">
+        <v>18</v>
+      </c>
+      <c r="I72" s="29">
+        <v>18</v>
+      </c>
+      <c r="J72" s="29">
+        <v>18</v>
+      </c>
+      <c r="K72" s="29">
+        <v>18</v>
+      </c>
+      <c r="L72" s="29">
+        <v>18</v>
+      </c>
+      <c r="M72" s="29">
+        <v>18</v>
+      </c>
+      <c r="N72" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>34</v>
       </c>
-      <c r="D72" t="str">
+      <c r="D73" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
         <v>Vivid</v>
       </c>
-      <c r="E72" t="str">
+      <c r="E73" t="str">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
         <v>LF</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F73" s="10">
         <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
-      <c r="K72" s="29"/>
-      <c r="L72" s="29"/>
-      <c r="M72" s="29"/>
-      <c r="N72" s="40"/>
-    </row>
-    <row r="73" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B73" s="1"/>
-      <c r="C73" t="s">
-        <v>36</v>
-      </c>
-      <c r="D73" t="str">
-        <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Align</v>
-      </c>
-      <c r="E73" t="e">
-        <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F73" s="10" t="e">
-        <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H73"/>
-      <c r="I73"/>
-      <c r="J73"/>
-      <c r="K73"/>
-      <c r="L73"/>
-      <c r="M73"/>
-      <c r="N73"/>
-    </row>
-    <row r="74" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="29">
+        <v>4</v>
+      </c>
+      <c r="I73" s="29">
+        <v>4</v>
+      </c>
+      <c r="J73" s="29">
+        <v>4</v>
+      </c>
+      <c r="K73" s="29">
+        <v>4</v>
+      </c>
+      <c r="L73" s="29">
+        <v>4</v>
+      </c>
+      <c r="M73" s="29">
+        <v>4</v>
+      </c>
+      <c r="N73" s="29">
+        <v>4</v>
+      </c>
+      <c r="O73" s="29"/>
+      <c r="P73" s="39"/>
+    </row>
+    <row r="74" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D74" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Hustler</v>
+        <v>Align</v>
       </c>
       <c r="E74" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9046,13 +9419,13 @@
       <c r="M74"/>
       <c r="N74"/>
     </row>
-    <row r="75" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D75" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9074,13 +9447,13 @@
       <c r="M75"/>
       <c r="N75"/>
     </row>
-    <row r="76" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D76" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9102,13 +9475,13 @@
       <c r="M76"/>
       <c r="N76"/>
     </row>
-    <row r="77" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D77" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9130,13 +9503,13 @@
       <c r="M77"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D78" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9158,13 +9531,13 @@
       <c r="M78"/>
       <c r="N78"/>
     </row>
-    <row r="79" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D79" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9186,13 +9559,13 @@
       <c r="M79"/>
       <c r="N79"/>
     </row>
-    <row r="80" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D80" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9220,7 +9593,7 @@
       </c>
       <c r="B81" s="1"/>
       <c r="C81" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D81" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9248,11 +9621,11 @@
       </c>
       <c r="B82" s="1"/>
       <c r="C82" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D82" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>MG</v>
+        <v>Hustler</v>
       </c>
       <c r="E82" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9276,7 +9649,7 @@
       </c>
       <c r="B83" s="1"/>
       <c r="C83" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D83" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9304,7 +9677,7 @@
       </c>
       <c r="B84" s="1"/>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D84" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9332,7 +9705,7 @@
       </c>
       <c r="B85" s="1"/>
       <c r="C85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D85" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9360,11 +9733,11 @@
       </c>
       <c r="B86" s="1"/>
       <c r="C86" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D86" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>TVN</v>
+        <v>MG</v>
       </c>
       <c r="E86" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9388,11 +9761,11 @@
       </c>
       <c r="B87" s="1"/>
       <c r="C87" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="D87" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Uncensored</v>
+        <v>TVN</v>
       </c>
       <c r="E87" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9416,7 +9789,7 @@
       </c>
       <c r="B88" s="1"/>
       <c r="C88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D88" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9444,11 +9817,11 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D89" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>UPC</v>
+        <v>Uncensored</v>
       </c>
       <c r="E89" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9472,11 +9845,11 @@
       </c>
       <c r="B90" s="1"/>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D90" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Vivid</v>
+        <v>UPC</v>
       </c>
       <c r="E90" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9495,12 +9868,12 @@
       <c r="N90"/>
     </row>
     <row r="91" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B91" s="3"/>
+      <c r="B91" s="1"/>
       <c r="C91" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D91" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9523,16 +9896,16 @@
       <c r="N91"/>
     </row>
     <row r="92" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B92" s="1"/>
+      <c r="A92" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B92" s="3"/>
       <c r="C92" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="D92" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>210DM</v>
+        <v>Vivid</v>
       </c>
       <c r="E92" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9556,7 +9929,7 @@
       </c>
       <c r="B93" s="1"/>
       <c r="C93" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D93" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9584,11 +9957,11 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="D94" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Align</v>
+        <v>210DM</v>
       </c>
       <c r="E94" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9612,7 +9985,7 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D95" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9640,7 +10013,7 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="D96" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9668,7 +10041,7 @@
       </c>
       <c r="B97" s="1"/>
       <c r="C97" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D97" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9696,7 +10069,7 @@
       </c>
       <c r="B98" s="1"/>
       <c r="C98" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="D98" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9724,7 +10097,7 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D99" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9752,7 +10125,7 @@
       </c>
       <c r="B100" s="1"/>
       <c r="C100" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="D100" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9780,7 +10153,7 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D101" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9808,7 +10181,7 @@
       </c>
       <c r="B102" s="1"/>
       <c r="C102" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="D102" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9836,7 +10209,7 @@
       </c>
       <c r="B103" s="1"/>
       <c r="C103" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D103" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9864,7 +10237,7 @@
       </c>
       <c r="B104" s="1"/>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="D104" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9892,7 +10265,7 @@
       </c>
       <c r="B105" s="1"/>
       <c r="C105" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D105" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9920,11 +10293,11 @@
       </c>
       <c r="B106" s="1"/>
       <c r="C106" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="D106" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Evil Angel</v>
+        <v>Align</v>
       </c>
       <c r="E106" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9948,7 +10321,7 @@
       </c>
       <c r="B107" s="1"/>
       <c r="C107" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="D107" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -9976,11 +10349,11 @@
       </c>
       <c r="B108" s="1"/>
       <c r="C108" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="D108" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Hustler</v>
+        <v>Evil Angel</v>
       </c>
       <c r="E108" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10004,7 +10377,7 @@
       </c>
       <c r="B109" s="1"/>
       <c r="C109" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D109" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10032,7 +10405,7 @@
       </c>
       <c r="B110" s="1"/>
       <c r="C110" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="D110" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10060,7 +10433,7 @@
       </c>
       <c r="B111" s="1"/>
       <c r="C111" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D111" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10088,7 +10461,7 @@
       </c>
       <c r="B112" s="1"/>
       <c r="C112" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D112" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10116,7 +10489,7 @@
       </c>
       <c r="B113" s="1"/>
       <c r="C113" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D113" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10144,7 +10517,7 @@
       </c>
       <c r="B114" s="1"/>
       <c r="C114" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="D114" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10172,7 +10545,7 @@
       </c>
       <c r="B115" s="1"/>
       <c r="C115" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D115" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10200,7 +10573,7 @@
       </c>
       <c r="B116" s="1"/>
       <c r="C116" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="D116" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10228,7 +10601,7 @@
       </c>
       <c r="B117" s="1"/>
       <c r="C117" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D117" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10256,7 +10629,7 @@
       </c>
       <c r="B118" s="1"/>
       <c r="C118" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="D118" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10284,7 +10657,7 @@
       </c>
       <c r="B119" s="1"/>
       <c r="C119" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D119" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10312,7 +10685,7 @@
       </c>
       <c r="B120" s="1"/>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D120" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10340,7 +10713,7 @@
       </c>
       <c r="B121" s="1"/>
       <c r="C121" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D121" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10368,7 +10741,7 @@
       </c>
       <c r="B122" s="1"/>
       <c r="C122" t="s">
-        <v>113</v>
+        <v>56</v>
       </c>
       <c r="D122" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10396,7 +10769,7 @@
       </c>
       <c r="B123" s="1"/>
       <c r="C123" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D123" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10424,7 +10797,7 @@
       </c>
       <c r="B124" s="1"/>
       <c r="C124" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="D124" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10452,7 +10825,7 @@
       </c>
       <c r="B125" s="1"/>
       <c r="C125" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D125" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10480,7 +10853,7 @@
       </c>
       <c r="B126" s="1"/>
       <c r="C126" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="D126" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10508,7 +10881,7 @@
       </c>
       <c r="B127" s="1"/>
       <c r="C127" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D127" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10536,7 +10909,7 @@
       </c>
       <c r="B128" s="1"/>
       <c r="C128" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="D128" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10564,7 +10937,7 @@
       </c>
       <c r="B129" s="1"/>
       <c r="C129" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D129" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10592,7 +10965,7 @@
       </c>
       <c r="B130" s="1"/>
       <c r="C130" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D130" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10620,7 +10993,7 @@
       </c>
       <c r="B131" s="1"/>
       <c r="C131" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D131" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10648,7 +11021,7 @@
       </c>
       <c r="B132" s="1"/>
       <c r="C132" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="D132" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10676,7 +11049,7 @@
       </c>
       <c r="B133" s="1"/>
       <c r="C133" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="D133" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10704,7 +11077,7 @@
       </c>
       <c r="B134" s="1"/>
       <c r="C134" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D134" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10732,7 +11105,7 @@
       </c>
       <c r="B135" s="1"/>
       <c r="C135" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D135" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10760,7 +11133,7 @@
       </c>
       <c r="B136" s="1"/>
       <c r="C136" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="D136" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10783,12 +11156,12 @@
       <c r="N136"/>
     </row>
     <row r="137" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B137" s="3"/>
+      <c r="B137" s="1"/>
       <c r="C137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D137" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10811,16 +11184,16 @@
       <c r="N137"/>
     </row>
     <row r="138" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="A138" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B138" s="1"/>
+      <c r="B138" s="3"/>
       <c r="C138" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="D138" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>MG</v>
+        <v>Hustler</v>
       </c>
       <c r="E138" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10844,7 +11217,7 @@
       </c>
       <c r="B139" s="1"/>
       <c r="C139" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D139" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10872,7 +11245,7 @@
       </c>
       <c r="B140" s="1"/>
       <c r="C140" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="D140" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10900,7 +11273,7 @@
       </c>
       <c r="B141" s="1"/>
       <c r="C141" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D141" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10928,7 +11301,7 @@
       </c>
       <c r="B142" s="1"/>
       <c r="C142" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="D142" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10956,7 +11329,7 @@
       </c>
       <c r="B143" s="1"/>
       <c r="C143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D143" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -10984,7 +11357,7 @@
       </c>
       <c r="B144" s="1"/>
       <c r="C144" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="D144" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11012,7 +11385,7 @@
       </c>
       <c r="B145" s="1"/>
       <c r="C145" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D145" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11040,7 +11413,7 @@
       </c>
       <c r="B146" s="1"/>
       <c r="C146" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="D146" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11068,7 +11441,7 @@
       </c>
       <c r="B147" s="1"/>
       <c r="C147" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="D147" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11096,7 +11469,7 @@
       </c>
       <c r="B148" s="1"/>
       <c r="C148" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="D148" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11124,7 +11497,7 @@
       </c>
       <c r="B149" s="1"/>
       <c r="C149" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D149" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11152,7 +11525,7 @@
       </c>
       <c r="B150" s="1"/>
       <c r="C150" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="D150" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11180,7 +11553,7 @@
       </c>
       <c r="B151" s="1"/>
       <c r="C151" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D151" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11208,7 +11581,7 @@
       </c>
       <c r="B152" s="1"/>
       <c r="C152" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="D152" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11236,7 +11609,7 @@
       </c>
       <c r="B153" s="1"/>
       <c r="C153" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D153" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11264,11 +11637,11 @@
       </c>
       <c r="B154" s="1"/>
       <c r="C154" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="D154" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>PB</v>
+        <v>MG</v>
       </c>
       <c r="E154" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11292,11 +11665,11 @@
       </c>
       <c r="B155" s="1"/>
       <c r="C155" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D155" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>TVN</v>
+        <v>PB</v>
       </c>
       <c r="E155" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11320,7 +11693,7 @@
       </c>
       <c r="B156" s="1"/>
       <c r="C156" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D156" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11348,7 +11721,7 @@
       </c>
       <c r="B157" s="1"/>
       <c r="C157" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D157" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11376,7 +11749,7 @@
       </c>
       <c r="B158" s="1"/>
       <c r="C158" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D158" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11404,7 +11777,7 @@
       </c>
       <c r="B159" s="1"/>
       <c r="C159" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D159" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11432,7 +11805,7 @@
       </c>
       <c r="B160" s="1"/>
       <c r="C160" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D160" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11460,7 +11833,7 @@
       </c>
       <c r="B161" s="1"/>
       <c r="C161" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="D161" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11488,7 +11861,7 @@
       </c>
       <c r="B162" s="1"/>
       <c r="C162" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D162" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11516,7 +11889,7 @@
       </c>
       <c r="B163" s="1"/>
       <c r="C163" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="D163" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11544,7 +11917,7 @@
       </c>
       <c r="B164" s="1"/>
       <c r="C164" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="D164" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11572,7 +11945,7 @@
       </c>
       <c r="B165" s="1"/>
       <c r="C165" t="s">
-        <v>129</v>
+        <v>64</v>
       </c>
       <c r="D165" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11600,7 +11973,7 @@
       </c>
       <c r="B166" s="1"/>
       <c r="C166" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D166" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11628,11 +12001,11 @@
       </c>
       <c r="B167" s="1"/>
       <c r="C167" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="D167" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Uncensored</v>
+        <v>TVN</v>
       </c>
       <c r="E167" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11656,7 +12029,7 @@
       </c>
       <c r="B168" s="1"/>
       <c r="C168" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D168" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11684,11 +12057,11 @@
       </c>
       <c r="B169" s="1"/>
       <c r="C169" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D169" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Vivid</v>
+        <v>Uncensored</v>
       </c>
       <c r="E169" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11712,7 +12085,7 @@
       </c>
       <c r="B170" s="1"/>
       <c r="C170" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D170" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11740,7 +12113,7 @@
       </c>
       <c r="B171" s="1"/>
       <c r="C171" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D171" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11768,7 +12141,7 @@
       </c>
       <c r="B172" s="1"/>
       <c r="C172" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D172" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11796,7 +12169,7 @@
       </c>
       <c r="B173" s="1"/>
       <c r="C173" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="D173" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11824,7 +12197,7 @@
       </c>
       <c r="B174" s="1"/>
       <c r="C174" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D174" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11852,7 +12225,7 @@
       </c>
       <c r="B175" s="1"/>
       <c r="C175" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D175" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11880,7 +12253,7 @@
       </c>
       <c r="B176" s="1"/>
       <c r="C176" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D176" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11908,7 +12281,7 @@
       </c>
       <c r="B177" s="1"/>
       <c r="C177" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="D177" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11936,7 +12309,7 @@
       </c>
       <c r="B178" s="1"/>
       <c r="C178" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D178" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11964,7 +12337,7 @@
       </c>
       <c r="B179" s="1"/>
       <c r="C179" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="D179" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -11992,7 +12365,7 @@
       </c>
       <c r="B180" s="1"/>
       <c r="C180" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D180" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12020,7 +12393,7 @@
       </c>
       <c r="B181" s="1"/>
       <c r="C181" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="D181" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12048,7 +12421,7 @@
       </c>
       <c r="B182" s="1"/>
       <c r="C182" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D182" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12076,7 +12449,7 @@
       </c>
       <c r="B183" s="1"/>
       <c r="C183" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="D183" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12104,7 +12477,7 @@
       </c>
       <c r="B184" s="1"/>
       <c r="C184" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="D184" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12132,7 +12505,7 @@
       </c>
       <c r="B185" s="1"/>
       <c r="C185" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D185" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12160,7 +12533,7 @@
       </c>
       <c r="B186" s="1"/>
       <c r="C186" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="D186" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12188,7 +12561,7 @@
       </c>
       <c r="B187" s="1"/>
       <c r="C187" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="D187" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12216,7 +12589,7 @@
       </c>
       <c r="B188" s="1"/>
       <c r="C188" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D188" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12244,7 +12617,7 @@
       </c>
       <c r="B189" s="1"/>
       <c r="C189" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="D189" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12272,7 +12645,7 @@
       </c>
       <c r="B190" s="1"/>
       <c r="C190" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D190" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12300,7 +12673,7 @@
       </c>
       <c r="B191" s="1"/>
       <c r="C191" t="s">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="D191" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12328,7 +12701,7 @@
       </c>
       <c r="B192" s="1"/>
       <c r="C192" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D192" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12356,7 +12729,7 @@
       </c>
       <c r="B193" s="1"/>
       <c r="C193" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="D193" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12384,7 +12757,7 @@
       </c>
       <c r="B194" s="1"/>
       <c r="C194" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="D194" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12412,7 +12785,7 @@
       </c>
       <c r="B195" s="1"/>
       <c r="C195" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="D195" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12440,7 +12813,7 @@
       </c>
       <c r="B196" s="1"/>
       <c r="C196" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D196" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12468,7 +12841,7 @@
       </c>
       <c r="B197" s="1"/>
       <c r="C197" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="D197" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12496,7 +12869,7 @@
       </c>
       <c r="B198" s="1"/>
       <c r="C198" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D198" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12524,7 +12897,7 @@
       </c>
       <c r="B199" s="1"/>
       <c r="C199" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
       <c r="D199" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12547,12 +12920,12 @@
       <c r="N199"/>
     </row>
     <row r="200" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
+      <c r="A200" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B200" s="3"/>
+      <c r="B200" s="1"/>
       <c r="C200" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D200" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12575,16 +12948,16 @@
       <c r="N200"/>
     </row>
     <row r="201" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B201" s="1"/>
+      <c r="A201" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B201" s="3"/>
       <c r="C201" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D201" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>210DM</v>
+        <v>Vivid</v>
       </c>
       <c r="E201" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12608,11 +12981,11 @@
       </c>
       <c r="B202" s="1"/>
       <c r="C202" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="D202" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Align</v>
+        <v>210DM</v>
       </c>
       <c r="E202" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12636,7 +13009,7 @@
       </c>
       <c r="B203" s="1"/>
       <c r="C203" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="D203" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12664,7 +13037,7 @@
       </c>
       <c r="B204" s="1"/>
       <c r="C204" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="D204" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12692,7 +13065,7 @@
       </c>
       <c r="B205" s="1"/>
       <c r="C205" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D205" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12720,11 +13093,11 @@
       </c>
       <c r="B206" s="1"/>
       <c r="C206" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D206" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Digital Playground</v>
+        <v>Align</v>
       </c>
       <c r="E206" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12748,7 +13121,7 @@
       </c>
       <c r="B207" s="1"/>
       <c r="C207" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D207" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12776,11 +13149,11 @@
       </c>
       <c r="B208" s="1"/>
       <c r="C208" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D208" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Hustler</v>
+        <v>Digital Playground</v>
       </c>
       <c r="E208" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12804,7 +13177,7 @@
       </c>
       <c r="B209" s="1"/>
       <c r="C209" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D209" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12832,7 +13205,7 @@
       </c>
       <c r="B210" s="1"/>
       <c r="C210" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D210" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12860,7 +13233,7 @@
       </c>
       <c r="B211" s="1"/>
       <c r="C211" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D211" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12888,7 +13261,7 @@
       </c>
       <c r="B212" s="1"/>
       <c r="C212" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="D212" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12916,7 +13289,7 @@
       </c>
       <c r="B213" s="1"/>
       <c r="C213" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D213" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12944,11 +13317,11 @@
       </c>
       <c r="B214" s="1"/>
       <c r="C214" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D214" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>MG</v>
+        <v>Hustler</v>
       </c>
       <c r="E214" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -12972,7 +13345,7 @@
       </c>
       <c r="B215" s="1"/>
       <c r="C215" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="D215" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13000,7 +13373,7 @@
       </c>
       <c r="B216" s="1"/>
       <c r="C216" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D216" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13028,7 +13401,7 @@
       </c>
       <c r="B217" s="1"/>
       <c r="C217" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D217" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13056,7 +13429,7 @@
       </c>
       <c r="B218" s="1"/>
       <c r="C218" t="s">
-        <v>151</v>
+        <v>28</v>
       </c>
       <c r="D218" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13084,7 +13457,7 @@
       </c>
       <c r="B219" s="1"/>
       <c r="C219" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D219" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13112,7 +13485,7 @@
       </c>
       <c r="B220" s="1"/>
       <c r="C220" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="D220" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13140,11 +13513,11 @@
       </c>
       <c r="B221" s="1"/>
       <c r="C221" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="D221" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>TVN</v>
+        <v>MG</v>
       </c>
       <c r="E221" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13168,7 +13541,7 @@
       </c>
       <c r="B222" s="1"/>
       <c r="C222" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="D222" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13196,7 +13569,7 @@
       </c>
       <c r="B223" s="1"/>
       <c r="C223" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="D223" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13224,7 +13597,7 @@
       </c>
       <c r="B224" s="1"/>
       <c r="C224" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="D224" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13252,7 +13625,7 @@
       </c>
       <c r="B225" s="1"/>
       <c r="C225" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D225" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13280,7 +13653,7 @@
       </c>
       <c r="B226" s="1"/>
       <c r="C226" t="s">
-        <v>143</v>
+        <v>12</v>
       </c>
       <c r="D226" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13308,7 +13681,7 @@
       </c>
       <c r="B227" s="1"/>
       <c r="C227" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="D227" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13336,7 +13709,7 @@
       </c>
       <c r="B228" s="1"/>
       <c r="C228" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="D228" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13364,7 +13737,7 @@
       </c>
       <c r="B229" s="1"/>
       <c r="C229" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="D229" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13392,7 +13765,7 @@
       </c>
       <c r="B230" s="1"/>
       <c r="C230" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="D230" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13420,11 +13793,11 @@
       </c>
       <c r="B231" s="1"/>
       <c r="C231" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D231" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>UPC</v>
+        <v>TVN</v>
       </c>
       <c r="E231" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13448,11 +13821,11 @@
       </c>
       <c r="B232" s="1"/>
       <c r="C232" t="s">
-        <v>6</v>
+        <v>149</v>
       </c>
       <c r="D232" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Vivid</v>
+        <v>UPC</v>
       </c>
       <c r="E232" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13476,7 +13849,7 @@
       </c>
       <c r="B233" s="1"/>
       <c r="C233" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D233" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13504,7 +13877,7 @@
       </c>
       <c r="B234" s="1"/>
       <c r="C234" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D234" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13532,7 +13905,7 @@
       </c>
       <c r="B235" s="1"/>
       <c r="C235" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D235" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13560,7 +13933,7 @@
       </c>
       <c r="B236" s="1"/>
       <c r="C236" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D236" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13588,7 +13961,7 @@
       </c>
       <c r="B237" s="1"/>
       <c r="C237" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D237" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13616,7 +13989,7 @@
       </c>
       <c r="B238" s="1"/>
       <c r="C238" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D238" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13639,16 +14012,16 @@
       <c r="N238"/>
     </row>
     <row r="239" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="2" t="s">
+      <c r="A239" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B239" s="3"/>
+      <c r="B239" s="1"/>
       <c r="C239" t="s">
-        <v>171</v>
+        <v>33</v>
       </c>
       <c r="D239" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>MG</v>
+        <v>Vivid</v>
       </c>
       <c r="E239" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13667,16 +14040,16 @@
       <c r="N239"/>
     </row>
     <row r="240" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B240" s="1"/>
+      <c r="A240" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B240" s="3"/>
       <c r="C240" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="D240" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>210DM</v>
+        <v>MG</v>
       </c>
       <c r="E240" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13700,11 +14073,11 @@
       </c>
       <c r="B241" s="1"/>
       <c r="C241" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="D241" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>360 AI</v>
+        <v>210DM</v>
       </c>
       <c r="E241" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13728,11 +14101,11 @@
       </c>
       <c r="B242" s="1"/>
       <c r="C242" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D242" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Align</v>
+        <v>360 AI</v>
       </c>
       <c r="E242" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13756,7 +14129,7 @@
       </c>
       <c r="B243" s="1"/>
       <c r="C243" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="D243" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13784,7 +14157,7 @@
       </c>
       <c r="B244" s="1"/>
       <c r="C244" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D244" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13812,7 +14185,7 @@
       </c>
       <c r="B245" s="1"/>
       <c r="C245" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D245" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13840,7 +14213,7 @@
       </c>
       <c r="B246" s="1"/>
       <c r="C246" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D246" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13868,7 +14241,7 @@
       </c>
       <c r="B247" s="1"/>
       <c r="C247" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D247" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13896,7 +14269,7 @@
       </c>
       <c r="B248" s="1"/>
       <c r="C248" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D248" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13924,11 +14297,11 @@
       </c>
       <c r="B249" s="1"/>
       <c r="C249" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D249" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Digital Playground</v>
+        <v>Align</v>
       </c>
       <c r="E249" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13952,11 +14325,11 @@
       </c>
       <c r="B250" s="1"/>
       <c r="C250" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="D250" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Evil Angel</v>
+        <v>Digital Playground</v>
       </c>
       <c r="E250" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -13980,11 +14353,11 @@
       </c>
       <c r="B251" s="1"/>
       <c r="C251" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="D251" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Hustler</v>
+        <v>Evil Angel</v>
       </c>
       <c r="E251" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14008,7 +14381,7 @@
       </c>
       <c r="B252" s="1"/>
       <c r="C252" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D252" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14036,7 +14409,7 @@
       </c>
       <c r="B253" s="1"/>
       <c r="C253" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="D253" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14064,7 +14437,7 @@
       </c>
       <c r="B254" s="1"/>
       <c r="C254" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D254" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14092,7 +14465,7 @@
       </c>
       <c r="B255" s="1"/>
       <c r="C255" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="D255" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14120,7 +14493,7 @@
       </c>
       <c r="B256" s="1"/>
       <c r="C256" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D256" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14148,7 +14521,7 @@
       </c>
       <c r="B257" s="1"/>
       <c r="C257" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D257" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14176,7 +14549,7 @@
       </c>
       <c r="B258" s="1"/>
       <c r="C258" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="D258" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14204,7 +14577,7 @@
       </c>
       <c r="B259" s="1"/>
       <c r="C259" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="D259" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14232,7 +14605,7 @@
       </c>
       <c r="B260" s="1"/>
       <c r="C260" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D260" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14260,7 +14633,7 @@
       </c>
       <c r="B261" s="1"/>
       <c r="C261" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D261" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14288,7 +14661,7 @@
       </c>
       <c r="B262" s="1"/>
       <c r="C262" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="D262" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14316,7 +14689,7 @@
       </c>
       <c r="B263" s="1"/>
       <c r="C263" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D263" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14339,12 +14712,12 @@
       <c r="N263"/>
     </row>
     <row r="264" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="3" t="s">
+      <c r="A264" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B264" s="3"/>
+      <c r="B264" s="1"/>
       <c r="C264" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D264" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14367,16 +14740,16 @@
       <c r="N264"/>
     </row>
     <row r="265" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
+      <c r="A265" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B265" s="1"/>
+      <c r="B265" s="3"/>
       <c r="C265" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D265" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>MG</v>
+        <v>Hustler</v>
       </c>
       <c r="E265" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14400,7 +14773,7 @@
       </c>
       <c r="B266" s="1"/>
       <c r="C266" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="D266" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14428,7 +14801,7 @@
       </c>
       <c r="B267" s="1"/>
       <c r="C267" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D267" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14456,7 +14829,7 @@
       </c>
       <c r="B268" s="1"/>
       <c r="C268" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D268" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14479,12 +14852,12 @@
       <c r="N268"/>
     </row>
     <row r="269" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="3" t="s">
+      <c r="A269" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B269" s="3"/>
+      <c r="B269" s="1"/>
       <c r="C269" t="s">
-        <v>151</v>
+        <v>28</v>
       </c>
       <c r="D269" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14507,12 +14880,12 @@
       <c r="N269"/>
     </row>
     <row r="270" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
+      <c r="A270" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B270" s="1"/>
+      <c r="B270" s="3"/>
       <c r="C270" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D270" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14540,7 +14913,7 @@
       </c>
       <c r="B271" s="1"/>
       <c r="C271" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="D271" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14568,7 +14941,7 @@
       </c>
       <c r="B272" s="1"/>
       <c r="C272" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D272" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14596,7 +14969,7 @@
       </c>
       <c r="B273" s="1"/>
       <c r="C273" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="D273" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14624,7 +14997,7 @@
       </c>
       <c r="B274" s="1"/>
       <c r="C274" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="D274" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14652,11 +15025,11 @@
       </c>
       <c r="B275" s="1"/>
       <c r="C275" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
       <c r="D275" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>MVP</v>
+        <v>MG</v>
       </c>
       <c r="E275" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14680,7 +15053,7 @@
       </c>
       <c r="B276" s="1"/>
       <c r="C276" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D276" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14708,7 +15081,7 @@
       </c>
       <c r="B277" s="1"/>
       <c r="C277" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D277" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14736,11 +15109,11 @@
       </c>
       <c r="B278" s="1"/>
       <c r="C278" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="D278" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>PB</v>
+        <v>MVP</v>
       </c>
       <c r="E278" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14764,11 +15137,11 @@
       </c>
       <c r="B279" s="1"/>
       <c r="C279" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="D279" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>TVN</v>
+        <v>PB</v>
       </c>
       <c r="E279" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14792,7 +15165,7 @@
       </c>
       <c r="B280" s="1"/>
       <c r="C280" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="D280" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14820,7 +15193,7 @@
       </c>
       <c r="B281" s="1"/>
       <c r="C281" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D281" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14848,7 +15221,7 @@
       </c>
       <c r="B282" s="1"/>
       <c r="C282" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D282" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14876,7 +15249,7 @@
       </c>
       <c r="B283" s="1"/>
       <c r="C283" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D283" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14904,7 +15277,7 @@
       </c>
       <c r="B284" s="1"/>
       <c r="C284" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D284" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14932,7 +15305,7 @@
       </c>
       <c r="B285" s="1"/>
       <c r="C285" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D285" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14960,7 +15333,7 @@
       </c>
       <c r="B286" s="1"/>
       <c r="C286" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D286" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -14988,7 +15361,7 @@
       </c>
       <c r="B287" s="1"/>
       <c r="C287" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="D287" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15016,7 +15389,7 @@
       </c>
       <c r="B288" s="1"/>
       <c r="C288" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="D288" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15044,11 +15417,11 @@
       </c>
       <c r="B289" s="1"/>
       <c r="C289" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D289" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
-        <v>Vivid</v>
+        <v>TVN</v>
       </c>
       <c r="E289" t="e">
         <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15072,7 +15445,7 @@
       </c>
       <c r="B290" s="1"/>
       <c r="C290" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D290" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15100,7 +15473,7 @@
       </c>
       <c r="B291" s="1"/>
       <c r="C291" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D291" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15128,7 +15501,7 @@
       </c>
       <c r="B292" s="1"/>
       <c r="C292" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D292" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15156,7 +15529,7 @@
       </c>
       <c r="B293" s="1"/>
       <c r="C293" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D293" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15184,7 +15557,7 @@
       </c>
       <c r="B294" s="1"/>
       <c r="C294" t="s">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="D294" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15212,7 +15585,7 @@
       </c>
       <c r="B295" s="1"/>
       <c r="C295" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="D295" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15240,7 +15613,7 @@
       </c>
       <c r="B296" s="1"/>
       <c r="C296" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D296" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15268,7 +15641,7 @@
       </c>
       <c r="B297" s="1"/>
       <c r="C297" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="D297" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15296,7 +15669,7 @@
       </c>
       <c r="B298" s="1"/>
       <c r="C298" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D298" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15324,7 +15697,7 @@
       </c>
       <c r="B299" s="1"/>
       <c r="C299" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D299" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15352,7 +15725,7 @@
       </c>
       <c r="B300" s="1"/>
       <c r="C300" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D300" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15380,7 +15753,7 @@
       </c>
       <c r="B301" s="1"/>
       <c r="C301" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
       <c r="D301" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15408,7 +15781,7 @@
       </c>
       <c r="B302" s="1"/>
       <c r="C302" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D302" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15436,7 +15809,7 @@
       </c>
       <c r="B303" s="1"/>
       <c r="C303" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D303" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15464,7 +15837,7 @@
       </c>
       <c r="B304" s="1"/>
       <c r="C304" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D304" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15492,7 +15865,7 @@
       </c>
       <c r="B305" s="1"/>
       <c r="C305" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="D305" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15520,7 +15893,7 @@
       </c>
       <c r="B306" s="1"/>
       <c r="C306" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="D306" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15543,12 +15916,12 @@
       <c r="N306"/>
     </row>
     <row r="307" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A307" s="2" t="s">
+      <c r="A307" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B307" s="3"/>
+      <c r="B307" s="1"/>
       <c r="C307" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D307" t="str">
         <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
@@ -15570,21 +15943,50 @@
       <c r="M307"/>
       <c r="N307"/>
     </row>
+    <row r="308" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B308" s="3"/>
+      <c r="C308" t="s">
+        <v>34</v>
+      </c>
+      <c r="D308" t="str">
+        <f>INDEX([1]network_ids!$C:$C,MATCH(titles_trend[[#This Row],[offering_rollup]],[1]network_ids!$E:$E,FALSE))</f>
+        <v>Vivid</v>
+      </c>
+      <c r="E308" t="e">
+        <f>INDEX([1]network_ids!$G:$G,MATCH(titles_trend[[#This Row],[offering]],[1]network_ids!$E:$E,FALSE))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F308" s="10" t="e">
+        <f>INDEX(Table3[hours],MATCH(titles_trend[[#This Row],[type]],Table3[type],FALSE))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H308"/>
+      <c r="I308"/>
+      <c r="J308"/>
+      <c r="K308"/>
+      <c r="L308"/>
+      <c r="M308"/>
+      <c r="N308"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D32 D34:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"MG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"MG"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="81" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -15593,9 +15995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15604,18 +16004,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B2" s="4">
         <v>160</v>
@@ -15627,7 +16027,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B3" s="5">
         <v>320</v>
@@ -15639,7 +16039,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B4" s="4">
         <v>80</v>
@@ -15651,7 +16051,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B5" s="4">
         <v>80</v>
@@ -15663,7 +16063,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B6" s="4">
         <v>80</v>
@@ -15675,7 +16075,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B7" s="4">
         <v>80</v>
@@ -15687,7 +16087,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B8" s="4">
         <v>20</v>
@@ -15699,7 +16099,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B9" s="4">
         <v>70</v>

</xml_diff>